<commit_message>
processos bag - com tempo de exec e programas
</commit_message>
<xml_diff>
--- a/Tempo de Execução - SpeedUp - Eficiencia.xlsx
+++ b/Tempo de Execução - SpeedUp - Eficiencia.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\romanofer\projects\paralela-primeiro-trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13005" windowHeight="6300"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="36">
   <si>
     <t>Caso Naive</t>
   </si>
@@ -164,7 +164,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,6 +192,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -255,13 +261,16 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -546,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,14 +579,14 @@
   <sheetData>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -681,42 +690,42 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D9" s="8"/>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="K11" s="9" t="s">
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="K11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="P11" s="9" t="s">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="P11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -797,12 +806,8 @@
         <v>1</v>
       </c>
       <c r="L13" s="5"/>
-      <c r="M13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
       <c r="P13" s="1">
         <v>1</v>
       </c>
@@ -846,26 +851,30 @@
       <c r="K14" s="1">
         <v>2</v>
       </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="1" t="e">
+      <c r="L14" s="5">
+        <v>1.911</v>
+      </c>
+      <c r="M14" s="1">
         <f>L13/L14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N14" s="1" t="e">
-        <f>L13/(K14*L14)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" ref="N14" si="0">M14*K13/K14</f>
+        <v>0</v>
       </c>
       <c r="P14" s="1">
         <v>2</v>
       </c>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="1" t="e">
-        <f>Q13/Q14</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S14" s="1" t="e">
-        <f>Q13/(P14*Q14)</f>
-        <v>#DIV/0!</v>
+      <c r="Q14" s="5">
+        <v>1.994</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" ref="R14:R15" si="1">Q13/Q14</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="1">
+        <f t="shared" ref="S14:S15" si="2">R14*P13/P14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -900,53 +909,57 @@
       <c r="K15" s="1">
         <v>4</v>
       </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="1" t="e">
-        <f>L13/L15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" s="1" t="e">
-        <f>M15/K15</f>
-        <v>#DIV/0!</v>
+      <c r="L15" s="6">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="M15" s="1">
+        <f>L14/L15</f>
+        <v>2.2041522491349483</v>
+      </c>
+      <c r="N15" s="1">
+        <f>M15*K14/K15</f>
+        <v>1.1020761245674742</v>
       </c>
       <c r="P15" s="1">
         <v>4</v>
       </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="1" t="e">
-        <f>Q13/Q15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S15" s="1" t="e">
-        <f>R15/P15</f>
-        <v>#DIV/0!</v>
+      <c r="Q15" s="6">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" si="1"/>
+        <v>2.0100806451612905</v>
+      </c>
+      <c r="S15" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0050403225806452</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="F18" s="9" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="F18" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="K18" s="9" t="s">
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="K18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="P18" s="9" t="s">
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="P18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -1021,12 +1034,8 @@
         <v>1</v>
       </c>
       <c r="L20" s="5"/>
-      <c r="M20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
       <c r="P20" s="1">
         <v>1</v>
       </c>
@@ -1070,26 +1079,30 @@
       <c r="K21" s="1">
         <v>2</v>
       </c>
-      <c r="L21" s="5"/>
-      <c r="M21" s="1" t="e">
+      <c r="L21" s="5">
+        <v>1.986</v>
+      </c>
+      <c r="M21" s="1">
         <f>L20/L21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N21" s="1" t="e">
-        <f>M21/K21</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <f t="shared" ref="N21:N22" si="3">M21*K20/K21</f>
+        <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>2</v>
       </c>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="1" t="e">
-        <f>Q20/Q21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S21" s="1" t="e">
-        <f>R21/P21</f>
-        <v>#DIV/0!</v>
+      <c r="Q21" s="5">
+        <v>2.371</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" ref="R21:R22" si="4">Q20/Q21</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="1">
+        <f t="shared" ref="S21:S22" si="5">R21*P20/P21</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1124,53 +1137,57 @@
       <c r="K22" s="1">
         <v>4</v>
       </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="1" t="e">
-        <f>L20/L22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" s="1" t="e">
-        <f>M22/K22</f>
-        <v>#DIV/0!</v>
+      <c r="L22" s="6">
+        <v>0.879</v>
+      </c>
+      <c r="M22" s="1">
+        <f>L21/L22</f>
+        <v>2.2593856655290101</v>
+      </c>
+      <c r="N22" s="1">
+        <f t="shared" si="3"/>
+        <v>1.1296928327645051</v>
       </c>
       <c r="P22" s="1">
         <v>4</v>
       </c>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="1" t="e">
-        <f>Q20/Q22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S22" s="1" t="e">
-        <f>R22/P22</f>
-        <v>#DIV/0!</v>
+      <c r="Q22" s="6">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4317948717948719</v>
+      </c>
+      <c r="S22" s="1">
+        <f t="shared" si="5"/>
+        <v>1.2158974358974359</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="F26" s="9" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="F26" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="K26" s="9" t="s">
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="K26" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="P26" s="9" t="s">
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="P26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1300,25 +1317,27 @@
       <c r="K29" s="1">
         <v>2</v>
       </c>
-      <c r="L29" s="5"/>
-      <c r="M29" s="1" t="e">
+      <c r="L29" s="5">
+        <v>2.0539999999999998</v>
+      </c>
+      <c r="M29" s="1">
         <f>L28/L29</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N29" s="1" t="e">
-        <f>M29/K29</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" ref="N29:N30" si="6">M29*K28/K29</f>
+        <v>0</v>
       </c>
       <c r="P29" s="1">
         <v>2</v>
       </c>
       <c r="Q29" s="5"/>
       <c r="R29" s="1" t="e">
-        <f>Q28/Q29</f>
+        <f t="shared" ref="R29:R30" si="7">Q28/Q29</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S29" s="1" t="e">
-        <f>R29/P29</f>
+        <f t="shared" ref="S29:S30" si="8">R29*P28/P29</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1354,53 +1373,55 @@
       <c r="K30" s="1">
         <v>4</v>
       </c>
-      <c r="L30" s="6"/>
-      <c r="M30" s="1" t="e">
-        <f>L28/L30</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N30" s="1" t="e">
-        <f>M30/K30</f>
-        <v>#DIV/0!</v>
+      <c r="L30" s="6">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="M30" s="1">
+        <f>L29/L30</f>
+        <v>2.2374727668845313</v>
+      </c>
+      <c r="N30" s="1">
+        <f>M30*K29/K30</f>
+        <v>1.1187363834422657</v>
       </c>
       <c r="P30" s="1">
         <v>4</v>
       </c>
       <c r="Q30" s="6"/>
       <c r="R30" s="1" t="e">
-        <f>Q28/Q30</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S30" s="1" t="e">
-        <f>R30/P30</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="F33" s="9" t="s">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="F33" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="K33" s="9" t="s">
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="K33" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="P33" s="9" t="s">
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="P33" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
@@ -1530,26 +1551,30 @@
       <c r="K36" s="1">
         <v>2</v>
       </c>
-      <c r="L36" s="5"/>
-      <c r="M36" s="1" t="e">
+      <c r="L36" s="5">
+        <v>2.1379999999999999</v>
+      </c>
+      <c r="M36" s="1">
         <f>L35/L36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N36" s="1" t="e">
-        <f>M36/K36</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="N36" s="1">
+        <f t="shared" ref="N36" si="9">M36*K35/K36</f>
+        <v>0</v>
       </c>
       <c r="P36" s="1">
         <v>2</v>
       </c>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="1" t="e">
-        <f>Q35/Q36</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S36" s="1" t="e">
-        <f>R36/P36</f>
-        <v>#DIV/0!</v>
+      <c r="Q36" s="5">
+        <v>2.278</v>
+      </c>
+      <c r="R36" s="1">
+        <f t="shared" ref="R36:R37" si="10">Q35/Q36</f>
+        <v>0</v>
+      </c>
+      <c r="S36" s="1">
+        <f t="shared" ref="S36:S37" si="11">R36*P35/P36</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -1584,53 +1609,57 @@
       <c r="K37" s="1">
         <v>4</v>
       </c>
-      <c r="L37" s="6"/>
-      <c r="M37" s="1" t="e">
-        <f>L35/L37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N37" s="1" t="e">
-        <f>M37/K37</f>
-        <v>#DIV/0!</v>
+      <c r="L37" s="6">
+        <v>1.012</v>
+      </c>
+      <c r="M37" s="1">
+        <f>L36/L37</f>
+        <v>2.1126482213438735</v>
+      </c>
+      <c r="N37" s="1">
+        <f>M37*K36/K37</f>
+        <v>1.0563241106719368</v>
       </c>
       <c r="P37" s="1">
         <v>4</v>
       </c>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="1" t="e">
-        <f>Q35/Q37</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S37" s="1" t="e">
-        <f>R37/P37</f>
-        <v>#DIV/0!</v>
+      <c r="Q37" s="6">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="R37" s="1">
+        <f t="shared" si="10"/>
+        <v>2.4054910242872229</v>
+      </c>
+      <c r="S37" s="1">
+        <f t="shared" si="11"/>
+        <v>1.2027455121436115</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="F40" s="9" t="s">
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="F40" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="K40" s="9" t="s">
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="K40" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="P40" s="9" t="s">
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="P40" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -1760,26 +1789,30 @@
       <c r="K43" s="1">
         <v>2</v>
       </c>
-      <c r="L43" s="5"/>
-      <c r="M43" s="1" t="e">
+      <c r="L43" s="5">
+        <v>2.101</v>
+      </c>
+      <c r="M43" s="1">
         <f>L42/L43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N43" s="1" t="e">
-        <f>M43/K43</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
+      </c>
+      <c r="N43" s="1">
+        <f t="shared" ref="N43" si="12">M43*K42/K43</f>
+        <v>0</v>
       </c>
       <c r="P43" s="1">
         <v>2</v>
       </c>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="1" t="e">
-        <f>Q42/Q43</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S43" s="1" t="e">
-        <f>R43/P43</f>
-        <v>#DIV/0!</v>
+      <c r="Q43" s="5">
+        <v>2.2719999999999998</v>
+      </c>
+      <c r="R43" s="1">
+        <f t="shared" ref="R43:R44" si="13">Q42/Q43</f>
+        <v>0</v>
+      </c>
+      <c r="S43" s="1">
+        <f t="shared" ref="S43:S44" si="14">R43*P42/P43</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -1814,42 +1847,34 @@
       <c r="K44" s="1">
         <v>4</v>
       </c>
-      <c r="L44" s="6"/>
-      <c r="M44" s="1" t="e">
-        <f>L42/L44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N44" s="1" t="e">
-        <f>M44/K44</f>
-        <v>#DIV/0!</v>
+      <c r="L44" s="6">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="M44" s="1">
+        <f>L43/L44</f>
+        <v>2.1794605809128633</v>
+      </c>
+      <c r="N44" s="1">
+        <f>M44*K43/K44</f>
+        <v>1.0897302904564317</v>
       </c>
       <c r="P44" s="1">
         <v>4</v>
       </c>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="1" t="e">
-        <f>Q42/Q44</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S44" s="1" t="e">
-        <f>R44/P44</f>
-        <v>#DIV/0!</v>
+      <c r="Q44" s="6">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="R44" s="1">
+        <f t="shared" si="13"/>
+        <v>2.2384236453201969</v>
+      </c>
+      <c r="S44" s="1">
+        <f t="shared" si="14"/>
+        <v>1.1192118226600984</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F40:I40"/>
     <mergeCell ref="P40:S40"/>
     <mergeCell ref="F9:L9"/>
     <mergeCell ref="P11:S11"/>
@@ -1861,6 +1886,18 @@
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K33:N33"/>
     <mergeCell ref="K40:N40"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A26:D26"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix bag of tasks efficiency
</commit_message>
<xml_diff>
--- a/Tempo de Execução - SpeedUp - Eficiencia.xlsx
+++ b/Tempo de Execução - SpeedUp - Eficiencia.xlsx
@@ -401,8 +401,8 @@
   </sheetPr>
   <dimension ref="A2:S51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W29" activeCellId="0" sqref="W29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,8 +763,8 @@
         <v>2.57516611295681</v>
       </c>
       <c r="N15" s="1" t="n">
-        <f aca="false">M15*K14/K15</f>
-        <v>1.28758305647841</v>
+        <f aca="false">M15/K15</f>
+        <v>0.643791528239203</v>
       </c>
       <c r="P15" s="1" t="n">
         <v>4</v>
@@ -777,8 +777,8 @@
         <v>2.41229141229141</v>
       </c>
       <c r="S15" s="1" t="n">
-        <f aca="false">R15*P14/P15</f>
-        <v>1.20614570614571</v>
+        <f aca="false">R15/P15</f>
+        <v>0.603072853072853</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -985,8 +985,8 @@
         <v>2.76626192541197</v>
       </c>
       <c r="N22" s="1" t="n">
-        <f aca="false">M22*K21/K22</f>
-        <v>1.38313096270598</v>
+        <f aca="false">M22/K22</f>
+        <v>0.691565481352993</v>
       </c>
       <c r="P22" s="1" t="n">
         <v>4</v>
@@ -1207,8 +1207,8 @@
         <v>2.50569297212407</v>
       </c>
       <c r="N30" s="1" t="n">
-        <f aca="false">M30*K29/K30</f>
-        <v>1.25284648606203</v>
+        <f aca="false">M30/K30</f>
+        <v>0.626423243031018</v>
       </c>
       <c r="P30" s="1" t="n">
         <v>4</v>
@@ -1431,8 +1431,8 @@
         <v>2.6343954248366</v>
       </c>
       <c r="N37" s="1" t="n">
-        <f aca="false">M37*K36/K37</f>
-        <v>1.3171977124183</v>
+        <f aca="false">M37/K37</f>
+        <v>0.65859885620915</v>
       </c>
       <c r="P37" s="1" t="n">
         <v>4</v>
@@ -1655,8 +1655,8 @@
         <v>2.82787930301742</v>
       </c>
       <c r="N44" s="1" t="n">
-        <f aca="false">M44*K43/K44</f>
-        <v>1.41393965150871</v>
+        <f aca="false">M44/K44</f>
+        <v>0.706969825754355</v>
       </c>
       <c r="P44" s="1" t="n">
         <v>4</v>

</xml_diff>